<commit_message>
Added failing tests for adjacency and target lists.
</commit_message>
<xml_diff>
--- a/ClueGame/ClueLayoutExcel.xlsx
+++ b/ClueGame/ClueLayoutExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\ClueGameProject\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="27">
   <si>
     <t>K</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>AL</t>
+  </si>
+  <si>
+    <t>Number of Doors: 12</t>
+  </si>
+  <si>
+    <t>White: test door directions (FileInitTests)</t>
+  </si>
+  <si>
+    <t>Purple: Test adjacency lists for room exits.</t>
+  </si>
+  <si>
+    <t>Orange: Test adjacency lists inside rooms.</t>
+  </si>
+  <si>
+    <t>Green: Test adjacency lists beside doorway.</t>
+  </si>
+  <si>
+    <t>Light Purple: Tests adjacency lists in walkway.</t>
+  </si>
+  <si>
+    <t>Light Blue: Test target list creation.</t>
   </si>
 </sst>
 </file>
@@ -99,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +151,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -143,18 +206,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -429,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +529,7 @@
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -483,7 +559,7 @@
       <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -690,7 +766,7 @@
       <c r="M4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="O4" s="2" t="s">
@@ -761,7 +837,7 @@
       <c r="M5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -811,10 +887,10 @@
       <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -829,7 +905,7 @@
       <c r="L6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -864,7 +940,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -983,10 +1059,10 @@
       <c r="P8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="4" t="s">
+      <c r="Q8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="S8" s="2" t="s">
@@ -1069,7 +1145,7 @@
       <c r="U9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="W9">
@@ -1083,7 +1159,7 @@
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1178,7 +1254,7 @@
       <c r="J11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -1270,7 +1346,7 @@
       <c r="Q12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="S12" s="2" t="s">
@@ -1299,7 +1375,7 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1370,13 +1446,13 @@
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1453,7 +1529,7 @@
       <c r="G15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="11" t="s">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1474,7 +1550,7 @@
       <c r="N15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="O15" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P15" s="1" t="s">
@@ -1545,7 +1621,7 @@
       <c r="N16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="7" t="s">
         <v>2</v>
       </c>
       <c r="P16" s="1" t="s">
@@ -1586,10 +1662,10 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1604,7 +1680,7 @@
       <c r="J17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1622,7 +1698,7 @@
       <c r="P17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="6" t="s">
         <v>15</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -1675,10 +1751,10 @@
       <c r="J18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -2000,7 +2076,7 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2042,7 +2118,7 @@
       <c r="N23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="11" t="s">
         <v>2</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2063,7 +2139,7 @@
       <c r="U23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="V23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="W23">
@@ -2136,6 +2212,41 @@
       </c>
       <c r="V24">
         <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>